<commit_message>
glms and spatial stats
</commit_message>
<xml_diff>
--- a/GLM/glm summary 8-21-2014.xlsx
+++ b/GLM/glm summary 8-21-2014.xlsx
@@ -10,13 +10,14 @@
     <sheet name="variables" sheetId="2" r:id="rId1"/>
     <sheet name="model.avg" sheetId="1" r:id="rId2"/>
     <sheet name="table for comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="table2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
   <si>
     <t>Estimate</t>
   </si>
@@ -523,6 +524,9 @@
   <si>
     <t>intercept only</t>
   </si>
+  <si>
+    <t>Nagelkerke adjusted</t>
+  </si>
 </sst>
 </file>
 
@@ -530,7 +534,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1078,7 +1082,7 @@
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1107,14 +1111,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1492,7 +1508,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD16"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="B2:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1829,7 +1845,9 @@
       <c r="A17" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
@@ -1913,7 +1931,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="J36" sqref="J36:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2378,7 +2396,7 @@
         <v>2.6886896999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -3574,7 +3592,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3590,28 +3608,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="21" customFormat="1" ht="39" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="28" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4001,4 +4019,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="31" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="29"/>
+      <c r="B1" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.27081430000000001</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.28861009999999998</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.4034528</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.26436779999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.2848271</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.3008459</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.42055749999999997</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.2471264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5.0889030000000002E-2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4.6345820000000003E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>7.6192640000000006E-2</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.17816090000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>8.8847999999999996E-2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>7.9894699999999999E-2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.13134709999999999</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.21264369999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="27" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.14275199999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.1056189</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.1948443</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.12643679999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.19638249999999999</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.14219760000000001</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.26232430000000001</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.18390799999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>